<commit_message>
WIP ... This looks like it could be painful to setup the table exactly how I want ... Possibly shelving it for now.
</commit_message>
<xml_diff>
--- a/Flashcard-Generator-Tests/Data/ExcelDataset1.xlsx
+++ b/Flashcard-Generator-Tests/Data/ExcelDataset1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwell\source\repos\Printable-Flashcard-Generator\Flashcard-Generator-Tests\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76F87E7-0448-4479-A6E8-01BC96C9C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C114E144-4D7A-4360-A952-8BC4FAF2E687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="2740" windowWidth="28800" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Question</t>
   </si>
@@ -49,6 +49,48 @@
   </si>
   <si>
     <t>answer3</t>
+  </si>
+  <si>
+    <t>question5</t>
+  </si>
+  <si>
+    <t>question6</t>
+  </si>
+  <si>
+    <t>question7</t>
+  </si>
+  <si>
+    <t>question8</t>
+  </si>
+  <si>
+    <t>question9</t>
+  </si>
+  <si>
+    <t>question10</t>
+  </si>
+  <si>
+    <t>question4</t>
+  </si>
+  <si>
+    <t>answer4</t>
+  </si>
+  <si>
+    <t>answer5</t>
+  </si>
+  <si>
+    <t>answer6</t>
+  </si>
+  <si>
+    <t>answer7</t>
+  </si>
+  <si>
+    <t>answer8</t>
+  </si>
+  <si>
+    <t>answer9</t>
+  </si>
+  <si>
+    <t>answer10</t>
   </si>
 </sst>
 </file>
@@ -366,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD67"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,6 +452,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>